<commit_message>
Commit more progress on stat analysis.
</commit_message>
<xml_diff>
--- a/project/analysis.xlsx
+++ b/project/analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="0" windowWidth="28460" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="0" windowWidth="28460" windowHeight="16700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2014" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Year</t>
   </si>
@@ -32,26 +32,6 @@
 Seed</t>
   </si>
   <si>
-    <t>Better
-1-Pt Ratio</t>
-  </si>
-  <si>
-    <t>Better
-2-Pt Ratio</t>
-  </si>
-  <si>
-    <t>Better
-3-Pt Ratio</t>
-  </si>
-  <si>
-    <t>Better
-Overtime Ratio</t>
-  </si>
-  <si>
-    <t>Lower Points
-Allowed</t>
-  </si>
-  <si>
     <t>More
 Wins</t>
   </si>
@@ -106,6 +86,74 @@
   <si>
     <t>More
 WAC</t>
+  </si>
+  <si>
+    <t>Less 1-Pt
+Games</t>
+  </si>
+  <si>
+    <t>More 1-Pt
+Wins</t>
+  </si>
+  <si>
+    <t>More 1-Pt
+Games</t>
+  </si>
+  <si>
+    <t>Less 1-Pt
+Wins</t>
+  </si>
+  <si>
+    <t>More 2-Pt
+Games</t>
+  </si>
+  <si>
+    <t>Less 2-Pt
+Games</t>
+  </si>
+  <si>
+    <t>More 2-Pt
+Wins</t>
+  </si>
+  <si>
+    <t>Less 2-Pt
+Wins</t>
+  </si>
+  <si>
+    <t>More 3-Pt
+Games</t>
+  </si>
+  <si>
+    <t>Less 3-Pt
+Games</t>
+  </si>
+  <si>
+    <t>More 3-Pt
+Wins</t>
+  </si>
+  <si>
+    <t>Less 3-Pt
+Wins</t>
+  </si>
+  <si>
+    <t>More OT
+Games</t>
+  </si>
+  <si>
+    <t>More OT
+Wins</t>
+  </si>
+  <si>
+    <t>Less OT
+Games</t>
+  </si>
+  <si>
+    <t>Less OT
+Wins</t>
+  </si>
+  <si>
+    <t>Higher Point
+Margin</t>
   </si>
 </sst>
 </file>
@@ -536,11 +584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W50"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -548,27 +596,39 @@
     <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.83203125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="8" style="1" customWidth="1"/>
-    <col min="20" max="20" width="7.83203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
+    <col min="9" max="11" width="12.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="8" style="1" customWidth="1"/>
+    <col min="29" max="29" width="7.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="8" style="1" customWidth="1"/>
+    <col min="32" max="32" width="7.83203125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="7.5" style="1" customWidth="1"/>
+    <col min="34" max="34" width="8" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="47" customHeight="1">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="47" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -579,67 +639,100 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="22" customHeight="1">
+    </row>
+    <row r="2" spans="1:34" ht="22" customHeight="1">
       <c r="A2" s="1">
         <v>2002</v>
       </c>
@@ -652,29 +745,80 @@
         <v>0.71186440677966101</v>
       </c>
       <c r="D2" s="4">
-        <f>26/48</f>
-        <v>0.54166666666666663</v>
+        <f>21/40</f>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4">
+        <f>21/36</f>
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4">
+        <f>30/48</f>
+        <v>0.625</v>
+      </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="K2" s="4">
+        <f>24/39</f>
+        <v>0.61538461538461542</v>
+      </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4">
+        <f>30/54</f>
+        <v>0.55555555555555558</v>
+      </c>
       <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="O2" s="4">
+        <f>23/45</f>
+        <v>0.51111111111111107</v>
+      </c>
       <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="Q2" s="4">
+        <f>31/54</f>
+        <v>0.57407407407407407</v>
+      </c>
       <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-    </row>
-    <row r="3" spans="1:23" ht="22" customHeight="1">
+      <c r="S2" s="4">
+        <f>23/42</f>
+        <v>0.54761904761904767</v>
+      </c>
+      <c r="T2" s="4">
+        <f>43/63</f>
+        <v>0.68253968253968256</v>
+      </c>
+      <c r="U2" s="4">
+        <f>40/62</f>
+        <v>0.64516129032258063</v>
+      </c>
+      <c r="V2" s="4">
+        <f>36/55</f>
+        <v>0.65454545454545454</v>
+      </c>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4">
+        <f>39/63</f>
+        <v>0.61904761904761907</v>
+      </c>
+      <c r="Y2" s="4">
+        <f>38/63</f>
+        <v>0.60317460317460314</v>
+      </c>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4">
+        <f>40/63</f>
+        <v>0.63492063492063489</v>
+      </c>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+    </row>
+    <row r="3" spans="1:34" ht="22" customHeight="1">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -696,8 +840,20 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
-    </row>
-    <row r="4" spans="1:23" ht="22" customHeight="1">
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+    </row>
+    <row r="4" spans="1:34" ht="22" customHeight="1">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -719,8 +875,20 @@
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
-    </row>
-    <row r="5" spans="1:23" ht="22" customHeight="1">
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+    </row>
+    <row r="5" spans="1:34" ht="22" customHeight="1">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -742,8 +910,20 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
-    </row>
-    <row r="6" spans="1:23" ht="22" customHeight="1">
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+    </row>
+    <row r="6" spans="1:34" ht="22" customHeight="1">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -765,8 +945,20 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-    </row>
-    <row r="7" spans="1:23" ht="22" customHeight="1">
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+    </row>
+    <row r="7" spans="1:34" ht="22" customHeight="1">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -788,8 +980,20 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="1:23" ht="22" customHeight="1">
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+    </row>
+    <row r="8" spans="1:34" ht="22" customHeight="1">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -811,8 +1015,20 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
-    </row>
-    <row r="9" spans="1:23" ht="22" customHeight="1">
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="4"/>
+    </row>
+    <row r="9" spans="1:34" ht="22" customHeight="1">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -834,8 +1050,20 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
-    </row>
-    <row r="10" spans="1:23" ht="22" customHeight="1">
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+    </row>
+    <row r="10" spans="1:34" ht="22" customHeight="1">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -857,8 +1085,20 @@
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
-    </row>
-    <row r="11" spans="1:23" ht="22" customHeight="1">
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="4"/>
+    </row>
+    <row r="11" spans="1:34" ht="22" customHeight="1">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -880,8 +1120,20 @@
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
-    </row>
-    <row r="12" spans="1:23" ht="22" customHeight="1">
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="4"/>
+    </row>
+    <row r="12" spans="1:34" ht="22" customHeight="1">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -903,8 +1155,20 @@
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-    </row>
-    <row r="13" spans="1:23" ht="22" customHeight="1">
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+    </row>
+    <row r="13" spans="1:34" ht="22" customHeight="1">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -926,8 +1190,20 @@
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
-    </row>
-    <row r="14" spans="1:23" ht="22" customHeight="1">
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="4"/>
+    </row>
+    <row r="14" spans="1:34" ht="22" customHeight="1">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -949,8 +1225,20 @@
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="1:23" ht="22" customHeight="1">
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="4"/>
+    </row>
+    <row r="15" spans="1:34" ht="22" customHeight="1">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -972,8 +1260,20 @@
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-    </row>
-    <row r="16" spans="1:23" ht="22" customHeight="1">
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="4"/>
+    </row>
+    <row r="16" spans="1:34" ht="22" customHeight="1">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -995,8 +1295,20 @@
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
-    </row>
-    <row r="17" spans="2:22" ht="22" customHeight="1">
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="4"/>
+    </row>
+    <row r="17" spans="2:34" ht="22" customHeight="1">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1018,8 +1330,20 @@
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
-    </row>
-    <row r="18" spans="2:22" ht="22" customHeight="1">
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+    </row>
+    <row r="18" spans="2:34" ht="22" customHeight="1">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1041,8 +1365,20 @@
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
-    </row>
-    <row r="19" spans="2:22" ht="22" customHeight="1">
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="4"/>
+    </row>
+    <row r="19" spans="2:34" ht="22" customHeight="1">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1064,8 +1400,20 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
-    </row>
-    <row r="20" spans="2:22" ht="22" customHeight="1">
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+    </row>
+    <row r="20" spans="2:34" ht="22" customHeight="1">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1087,8 +1435,20 @@
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-    </row>
-    <row r="21" spans="2:22" ht="22" customHeight="1">
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+    </row>
+    <row r="21" spans="2:34" ht="22" customHeight="1">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1110,8 +1470,20 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-    </row>
-    <row r="22" spans="2:22" ht="22" customHeight="1">
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+    </row>
+    <row r="22" spans="2:34" ht="22" customHeight="1">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1133,8 +1505,20 @@
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-    </row>
-    <row r="23" spans="2:22" ht="22" customHeight="1">
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+    </row>
+    <row r="23" spans="2:34" ht="22" customHeight="1">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1156,8 +1540,20 @@
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
-    </row>
-    <row r="24" spans="2:22" ht="22" customHeight="1">
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4"/>
+    </row>
+    <row r="24" spans="2:34" ht="22" customHeight="1">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1179,8 +1575,20 @@
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-    </row>
-    <row r="25" spans="2:22" ht="22" customHeight="1">
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+      <c r="AG24" s="4"/>
+      <c r="AH24" s="4"/>
+    </row>
+    <row r="25" spans="2:34" ht="22" customHeight="1">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1202,8 +1610,20 @@
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
-    </row>
-    <row r="26" spans="2:22" ht="22" customHeight="1">
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="4"/>
+    </row>
+    <row r="26" spans="2:34" ht="22" customHeight="1">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1225,8 +1645,20 @@
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-    </row>
-    <row r="27" spans="2:22" ht="22" customHeight="1">
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+    </row>
+    <row r="27" spans="2:34" ht="22" customHeight="1">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1248,8 +1680,20 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
-    </row>
-    <row r="28" spans="2:22" ht="22" customHeight="1">
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+    </row>
+    <row r="28" spans="2:34" ht="22" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1271,8 +1715,20 @@
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
-    </row>
-    <row r="29" spans="2:22" ht="22" customHeight="1">
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="4"/>
+    </row>
+    <row r="29" spans="2:34" ht="22" customHeight="1">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1294,8 +1750,20 @@
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
-    </row>
-    <row r="30" spans="2:22" ht="22" customHeight="1">
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+    </row>
+    <row r="30" spans="2:34" ht="22" customHeight="1">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1317,8 +1785,20 @@
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
-    </row>
-    <row r="31" spans="2:22" ht="22" customHeight="1">
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+    </row>
+    <row r="31" spans="2:34" ht="22" customHeight="1">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1340,8 +1820,20 @@
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
-    </row>
-    <row r="32" spans="2:22" ht="22" customHeight="1">
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4"/>
+      <c r="AF31" s="4"/>
+      <c r="AG31" s="4"/>
+      <c r="AH31" s="4"/>
+    </row>
+    <row r="32" spans="2:34" ht="22" customHeight="1">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1363,8 +1855,20 @@
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
-    </row>
-    <row r="33" spans="2:22" ht="22" customHeight="1">
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="4"/>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="4"/>
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="4"/>
+    </row>
+    <row r="33" spans="2:34" ht="22" customHeight="1">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1386,8 +1890,20 @@
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
-    </row>
-    <row r="34" spans="2:22" ht="22" customHeight="1">
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="4"/>
+    </row>
+    <row r="34" spans="2:34" ht="22" customHeight="1">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1409,8 +1925,20 @@
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
-    </row>
-    <row r="35" spans="2:22" ht="22" customHeight="1">
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="4"/>
+    </row>
+    <row r="35" spans="2:34" ht="22" customHeight="1">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -1432,8 +1960,20 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
-    </row>
-    <row r="36" spans="2:22" ht="22" customHeight="1">
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
+      <c r="AC35" s="4"/>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="4"/>
+    </row>
+    <row r="36" spans="2:34" ht="22" customHeight="1">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1455,8 +1995,20 @@
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
-    </row>
-    <row r="37" spans="2:22" ht="22" customHeight="1">
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4"/>
+      <c r="AF36" s="4"/>
+      <c r="AG36" s="4"/>
+      <c r="AH36" s="4"/>
+    </row>
+    <row r="37" spans="2:34" ht="22" customHeight="1">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -1478,8 +2030,20 @@
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
-    </row>
-    <row r="38" spans="2:22" ht="22" customHeight="1">
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="4"/>
+      <c r="AD37" s="4"/>
+      <c r="AE37" s="4"/>
+      <c r="AF37" s="4"/>
+      <c r="AG37" s="4"/>
+      <c r="AH37" s="4"/>
+    </row>
+    <row r="38" spans="2:34" ht="22" customHeight="1">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1501,8 +2065,20 @@
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
-    </row>
-    <row r="39" spans="2:22" ht="22" customHeight="1">
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+      <c r="AB38" s="4"/>
+      <c r="AC38" s="4"/>
+      <c r="AD38" s="4"/>
+      <c r="AE38" s="4"/>
+      <c r="AF38" s="4"/>
+      <c r="AG38" s="4"/>
+      <c r="AH38" s="4"/>
+    </row>
+    <row r="39" spans="2:34" ht="22" customHeight="1">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -1524,8 +2100,20 @@
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
-    </row>
-    <row r="40" spans="2:22" ht="22" customHeight="1">
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+      <c r="AB39" s="4"/>
+      <c r="AC39" s="4"/>
+      <c r="AD39" s="4"/>
+      <c r="AE39" s="4"/>
+      <c r="AF39" s="4"/>
+      <c r="AG39" s="4"/>
+      <c r="AH39" s="4"/>
+    </row>
+    <row r="40" spans="2:34" ht="22" customHeight="1">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -1547,8 +2135,20 @@
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
-    </row>
-    <row r="41" spans="2:22" ht="22" customHeight="1">
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4"/>
+      <c r="AB40" s="4"/>
+      <c r="AC40" s="4"/>
+      <c r="AD40" s="4"/>
+      <c r="AE40" s="4"/>
+      <c r="AF40" s="4"/>
+      <c r="AG40" s="4"/>
+      <c r="AH40" s="4"/>
+    </row>
+    <row r="41" spans="2:34" ht="22" customHeight="1">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -1570,8 +2170,20 @@
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
-    </row>
-    <row r="42" spans="2:22" ht="22" customHeight="1">
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="4"/>
+      <c r="AE41" s="4"/>
+      <c r="AF41" s="4"/>
+      <c r="AG41" s="4"/>
+      <c r="AH41" s="4"/>
+    </row>
+    <row r="42" spans="2:34" ht="22" customHeight="1">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -1593,8 +2205,20 @@
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
       <c r="V42" s="4"/>
-    </row>
-    <row r="43" spans="2:22" ht="22" customHeight="1">
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="4"/>
+      <c r="AE42" s="4"/>
+      <c r="AF42" s="4"/>
+      <c r="AG42" s="4"/>
+      <c r="AH42" s="4"/>
+    </row>
+    <row r="43" spans="2:34" ht="22" customHeight="1">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -1616,8 +2240,20 @@
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
-    </row>
-    <row r="44" spans="2:22" ht="22" customHeight="1">
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="4"/>
+      <c r="AE43" s="4"/>
+      <c r="AF43" s="4"/>
+      <c r="AG43" s="4"/>
+      <c r="AH43" s="4"/>
+    </row>
+    <row r="44" spans="2:34" ht="22" customHeight="1">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -1639,8 +2275,20 @@
       <c r="T44" s="4"/>
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
-    </row>
-    <row r="45" spans="2:22" ht="22" customHeight="1">
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+      <c r="AC44" s="4"/>
+      <c r="AD44" s="4"/>
+      <c r="AE44" s="4"/>
+      <c r="AF44" s="4"/>
+      <c r="AG44" s="4"/>
+      <c r="AH44" s="4"/>
+    </row>
+    <row r="45" spans="2:34" ht="22" customHeight="1">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -1662,8 +2310,20 @@
       <c r="T45" s="4"/>
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
-    </row>
-    <row r="46" spans="2:22" ht="22" customHeight="1">
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="4"/>
+      <c r="AD45" s="4"/>
+      <c r="AE45" s="4"/>
+      <c r="AF45" s="4"/>
+      <c r="AG45" s="4"/>
+      <c r="AH45" s="4"/>
+    </row>
+    <row r="46" spans="2:34" ht="22" customHeight="1">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -1685,8 +2345,20 @@
       <c r="T46" s="4"/>
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
-    </row>
-    <row r="47" spans="2:22" ht="22" customHeight="1">
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="4"/>
+      <c r="AF46" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="4"/>
+    </row>
+    <row r="47" spans="2:34" ht="22" customHeight="1">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -1708,8 +2380,20 @@
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
-    </row>
-    <row r="48" spans="2:22" ht="22" customHeight="1">
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
+      <c r="AC47" s="4"/>
+      <c r="AD47" s="4"/>
+      <c r="AE47" s="4"/>
+      <c r="AF47" s="4"/>
+      <c r="AG47" s="4"/>
+      <c r="AH47" s="4"/>
+    </row>
+    <row r="48" spans="2:34" ht="22" customHeight="1">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -1731,8 +2415,20 @@
       <c r="T48" s="4"/>
       <c r="U48" s="4"/>
       <c r="V48" s="4"/>
-    </row>
-    <row r="49" spans="2:22" ht="22" customHeight="1">
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="4"/>
+      <c r="AE48" s="4"/>
+      <c r="AF48" s="4"/>
+      <c r="AG48" s="4"/>
+      <c r="AH48" s="4"/>
+    </row>
+    <row r="49" spans="2:34" ht="22" customHeight="1">
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -1754,8 +2450,20 @@
       <c r="T49" s="4"/>
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
-    </row>
-    <row r="50" spans="2:22" ht="22" customHeight="1">
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4"/>
+      <c r="AE49" s="4"/>
+      <c r="AF49" s="4"/>
+      <c r="AG49" s="4"/>
+      <c r="AH49" s="4"/>
+    </row>
+    <row r="50" spans="2:34" ht="22" customHeight="1">
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -1777,6 +2485,18 @@
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="4"/>
+      <c r="AE50" s="4"/>
+      <c r="AF50" s="4"/>
+      <c r="AG50" s="4"/>
+      <c r="AH50" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>